<commit_message>
splitting seders from divrei hayamim backwards
</commit_message>
<xml_diff>
--- a/tests/notMesora.xlsx
+++ b/tests/notMesora.xlsx
@@ -88,7 +88,7 @@
     <t>4/10</t>
   </si>
   <si>
-    <t>יהושע ח א</t>
+    <t>יהושע ח לג</t>
   </si>
   <si>
     <t>כט תשרי</t>
@@ -97,7 +97,7 @@
     <t>5/10</t>
   </si>
   <si>
-    <t>יהושע ח לג</t>
+    <t>יהושע י ח</t>
   </si>
   <si>
     <t>ל תשרי</t>
@@ -106,7 +106,7 @@
     <t>6/10</t>
   </si>
   <si>
-    <t>יהושע י ח</t>
+    <t>יהושע י מב</t>
   </si>
   <si>
     <t>א חשון</t>
@@ -115,7 +115,7 @@
     <t>7/10</t>
   </si>
   <si>
-    <t>יהושע י מב</t>
+    <t>יהושע יג א</t>
   </si>
   <si>
     <t>ב חשון</t>
@@ -124,7 +124,7 @@
     <t>8/10</t>
   </si>
   <si>
-    <t>יהושע יג א</t>
+    <t>יהושע יד טו</t>
   </si>
   <si>
     <t>ג חשון</t>
@@ -142,7 +142,7 @@
     <t>10/10</t>
   </si>
   <si>
-    <t>יהושע יד טו</t>
+    <t>יהושע יז ד</t>
   </si>
   <si>
     <t>ה חשון</t>
@@ -151,7 +151,7 @@
     <t>11/10</t>
   </si>
   <si>
-    <t>יהושע יז ד</t>
+    <t>יהושע יח כח</t>
   </si>
   <si>
     <t>ו חשון</t>
@@ -160,7 +160,7 @@
     <t>12/10</t>
   </si>
   <si>
-    <t>יהושע יח כח</t>
+    <t>יהושע יט נא</t>
   </si>
   <si>
     <t>ז חשון</t>
@@ -169,7 +169,7 @@
     <t>13/10</t>
   </si>
   <si>
-    <t>יהושע יט נא</t>
+    <t>יהושע כא מא</t>
   </si>
   <si>
     <t>ח חשון</t>
@@ -178,7 +178,7 @@
     <t>14/10</t>
   </si>
   <si>
-    <t>יהושע כא מא</t>
+    <t>יהושע כב לד</t>
   </si>
   <si>
     <t>ט חשון</t>
@@ -187,7 +187,7 @@
     <t>15/10</t>
   </si>
   <si>
-    <t>יהושע כב לד</t>
+    <t>שופטים א א</t>
   </si>
   <si>
     <t>י חשון</t>
@@ -205,7 +205,7 @@
     <t>17/10</t>
   </si>
   <si>
-    <t>שופטים א א</t>
+    <t>שופטים ב ז</t>
   </si>
   <si>
     <t>יב חשון</t>
@@ -214,7 +214,7 @@
     <t>18/10</t>
   </si>
   <si>
-    <t>שופטים ב ז</t>
+    <t>שופטים ג לא</t>
   </si>
   <si>
     <t>יג חשון</t>
@@ -223,7 +223,7 @@
     <t>19/10</t>
   </si>
   <si>
-    <t>שופטים ג לא</t>
+    <t>שופטים ה לא</t>
   </si>
   <si>
     <t>יד חשון</t>
@@ -232,7 +232,7 @@
     <t>20/10</t>
   </si>
   <si>
-    <t>שופטים ה לא</t>
+    <t>שופטים ו מ</t>
   </si>
   <si>
     <t>טו חשון</t>
@@ -241,7 +241,7 @@
     <t>21/10</t>
   </si>
   <si>
-    <t>שופטים ו מ</t>
+    <t>שופטים ח ג</t>
   </si>
   <si>
     <t>טז חשון</t>
@@ -250,7 +250,7 @@
     <t>22/10</t>
   </si>
   <si>
-    <t>שופטים ח ג</t>
+    <t>שופטים ט ז</t>
   </si>
   <si>
     <t>יז חשון</t>
@@ -268,7 +268,7 @@
     <t>24/10</t>
   </si>
   <si>
-    <t>שופטים ט ז</t>
+    <t>שופטים י א</t>
   </si>
   <si>
     <t>יט חשון</t>
@@ -277,7 +277,7 @@
     <t>25/10</t>
   </si>
   <si>
-    <t>שופטים י א</t>
+    <t>שופטים יא לב</t>
   </si>
   <si>
     <t>כ חשון</t>
@@ -286,7 +286,7 @@
     <t>26/10</t>
   </si>
   <si>
-    <t>שופטים יא לב</t>
+    <t>שופטים יג כד</t>
   </si>
   <si>
     <t>כא חשון</t>
@@ -295,7 +295,7 @@
     <t>27/10</t>
   </si>
   <si>
-    <t>שופטים יג כד</t>
+    <t>שופטים טז ג</t>
   </si>
   <si>
     <t>כב חשון</t>
@@ -304,7 +304,7 @@
     <t>28/10</t>
   </si>
   <si>
-    <t>שופטים טז ג</t>
+    <t>שופטים יח ו</t>
   </si>
   <si>
     <t>כג חשון</t>
@@ -313,7 +313,7 @@
     <t>29/10</t>
   </si>
   <si>
-    <t>שופטים יח ו</t>
+    <t>שופטים יט כ</t>
   </si>
   <si>
     <t>כד חשון</t>
@@ -331,7 +331,7 @@
     <t>31/10</t>
   </si>
   <si>
-    <t>שופטים יט כ</t>
+    <t>שופטים כ כז</t>
   </si>
   <si>
     <t>כו חשון</t>
@@ -340,7 +340,7 @@
     <t>1/11</t>
   </si>
   <si>
-    <t>שופטים כ כז</t>
+    <t>שמו'א א א</t>
   </si>
   <si>
     <t>כז חשון</t>
@@ -349,7 +349,7 @@
     <t>2/11</t>
   </si>
   <si>
-    <t>שמו'א א א</t>
+    <t>שמו'א ב י</t>
   </si>
   <si>
     <t>כח חשון</t>
@@ -358,7 +358,7 @@
     <t>3/11</t>
   </si>
   <si>
-    <t>שמו'א ב י</t>
+    <t>שמו'א ג כ</t>
   </si>
   <si>
     <t>כט חשון</t>
@@ -367,7 +367,7 @@
     <t>4/11</t>
   </si>
   <si>
-    <t>שמו'א ג כ</t>
+    <t>שמו'א ו יד</t>
   </si>
   <si>
     <t>א כסלו</t>
@@ -376,7 +376,7 @@
     <t>5/11</t>
   </si>
   <si>
-    <t>שמו'א ו יד</t>
+    <t>שמו'א ט ב</t>
   </si>
   <si>
     <t>ב כסלו</t>
@@ -394,7 +394,7 @@
     <t>7/11</t>
   </si>
   <si>
-    <t>שמו'א ט ב</t>
+    <t>שמו'א י כד</t>
   </si>
   <si>
     <t>ד כסלו</t>
@@ -403,7 +403,7 @@
     <t>8/11</t>
   </si>
   <si>
-    <t>שמו'א י כד</t>
+    <t>שמו'א יב כב</t>
   </si>
   <si>
     <t>ה כסלו</t>
@@ -412,7 +412,7 @@
     <t>9/11</t>
   </si>
   <si>
-    <t>שמו'א יב כב</t>
+    <t>שמו'א יד כג</t>
   </si>
   <si>
     <t>ו כסלו</t>
@@ -421,7 +421,7 @@
     <t>10/11</t>
   </si>
   <si>
-    <t>שמו'א יד כג</t>
+    <t>שמו'א טו יז</t>
   </si>
   <si>
     <t>ז כסלו</t>
@@ -430,7 +430,7 @@
     <t>11/11</t>
   </si>
   <si>
-    <t>שמו'א טו יז</t>
+    <t>שמו'א טז יח</t>
   </si>
   <si>
     <t>ח כסלו</t>
@@ -439,7 +439,7 @@
     <t>12/11</t>
   </si>
   <si>
-    <t>שמו'א טז יח</t>
+    <t>שמו'א יז לז</t>
   </si>
   <si>
     <t>ט כסלו</t>
@@ -457,7 +457,7 @@
     <t>14/11</t>
   </si>
   <si>
-    <t>שמו'א יז לז</t>
+    <t>שמו'א יח יד</t>
   </si>
   <si>
     <t>יא כסלו</t>
@@ -466,7 +466,7 @@
     <t>15/11</t>
   </si>
   <si>
-    <t>שמו'א יח יד</t>
+    <t>שמו'א כ ד</t>
   </si>
   <si>
     <t>יב כסלו</t>
@@ -475,7 +475,7 @@
     <t>16/11</t>
   </si>
   <si>
-    <t>שמו'א כ ד</t>
+    <t>שמו'א כ מב</t>
   </si>
   <si>
     <t>יג כסלו</t>
@@ -484,7 +484,7 @@
     <t>17/11</t>
   </si>
   <si>
-    <t>שמו'א כ מב</t>
+    <t>שמו'א כג ד</t>
   </si>
   <si>
     <t>יד כסלו</t>
@@ -493,7 +493,7 @@
     <t>18/11</t>
   </si>
   <si>
-    <t>שמו'א כג ד</t>
+    <t>שמו'א כד כ</t>
   </si>
   <si>
     <t>טו כסלו</t>
@@ -502,7 +502,7 @@
     <t>19/11</t>
   </si>
   <si>
-    <t>שמו'א כד כ</t>
+    <t>שמו'א כה לג</t>
   </si>
   <si>
     <t>טז כסלו</t>
@@ -520,7 +520,7 @@
     <t>21/11</t>
   </si>
   <si>
-    <t>שמו'א כה לג</t>
+    <t>שמו'א כו כה</t>
   </si>
   <si>
     <t>יח כסלו</t>
@@ -529,7 +529,7 @@
     <t>22/11</t>
   </si>
   <si>
-    <t>שמו'א כו כה</t>
+    <t>שמו'א כח כד</t>
   </si>
   <si>
     <t>יט כסלו</t>
@@ -538,7 +538,7 @@
     <t>23/11</t>
   </si>
   <si>
-    <t>שמו'א כח כד</t>
+    <t>שמו'א ל כה</t>
   </si>
   <si>
     <t>כ כסלו</t>
@@ -547,7 +547,7 @@
     <t>24/11</t>
   </si>
   <si>
-    <t>שמו'א ל כה</t>
+    <t>שמו'ב ב ז</t>
   </si>
   <si>
     <t>כא כסלו</t>
@@ -556,7 +556,7 @@
     <t>25/11</t>
   </si>
   <si>
-    <t>שמו'ב ב ז</t>
+    <t>שמו'ב ג כא</t>
   </si>
   <si>
     <t>כב כסלו</t>
@@ -565,7 +565,7 @@
     <t>26/11</t>
   </si>
   <si>
-    <t>שמו'ב ג כא</t>
+    <t>שמו'ב ה י</t>
   </si>
   <si>
     <t>כג כסלו</t>
@@ -583,7 +583,7 @@
     <t>28/11</t>
   </si>
   <si>
-    <t>שמו'ב ה י</t>
+    <t>שמו'ב ז טז</t>
   </si>
   <si>
     <t>כה כסלו</t>
@@ -595,7 +595,7 @@
     <t>חנוכה</t>
   </si>
   <si>
-    <t>שמו'ב ז טז</t>
+    <t>שמו'ב י יג</t>
   </si>
   <si>
     <t>כו כסלו</t>
@@ -604,7 +604,7 @@
     <t>30/11</t>
   </si>
   <si>
-    <t>שמו'ב י יג</t>
+    <t>שמו'ב יב יג</t>
   </si>
   <si>
     <t>כז כסלו</t>
@@ -613,7 +613,7 @@
     <t>1/12</t>
   </si>
   <si>
-    <t>שמו'ב יב יג</t>
+    <t>שמו'ב יג כה</t>
   </si>
   <si>
     <t>כח כסלו</t>
@@ -622,7 +622,7 @@
     <t>2/12</t>
   </si>
   <si>
-    <t>שמו'ב יג כה</t>
+    <t>שמו'ב יד לג</t>
   </si>
   <si>
     <t>כט כסלו</t>
@@ -631,7 +631,7 @@
     <t>3/12</t>
   </si>
   <si>
-    <t>שמו'ב יד לג</t>
+    <t>שמו'ב טו לז</t>
   </si>
   <si>
     <t>ל כסלו</t>
@@ -649,7 +649,7 @@
     <t>5/12</t>
   </si>
   <si>
-    <t>שמו'ב טו לז</t>
+    <t>שמו'ב יז כ</t>
   </si>
   <si>
     <t>ב טבת</t>
@@ -658,7 +658,7 @@
     <t>6/12</t>
   </si>
   <si>
-    <t>שמו'ב יז כ</t>
+    <t>שמו'ב יח כז</t>
   </si>
   <si>
     <t>ג טבת</t>
@@ -667,7 +667,7 @@
     <t>7/12</t>
   </si>
   <si>
-    <t>שמו'ב יח כז</t>
+    <t>שמו'ב יט מ</t>
   </si>
   <si>
     <t>ד טבת</t>
@@ -676,7 +676,7 @@
     <t>8/12</t>
   </si>
   <si>
-    <t>שמו'ב יט מ</t>
+    <t>שמו'ב כא ז</t>
   </si>
   <si>
     <t>ה טבת</t>
@@ -685,7 +685,7 @@
     <t>9/12</t>
   </si>
   <si>
-    <t>שמו'ב כא ז</t>
+    <t>שמו'ב כב נא</t>
   </si>
   <si>
     <t>ו טבת</t>
@@ -694,7 +694,7 @@
     <t>10/12</t>
   </si>
   <si>
-    <t>שמו'ב כב נא</t>
+    <t>מלכ'א א א</t>
   </si>
   <si>
     <t>ז טבת</t>
@@ -712,7 +712,7 @@
     <t>12/12</t>
   </si>
   <si>
-    <t>מלכ'א א א</t>
+    <t>מלכ'א א מח</t>
   </si>
   <si>
     <t>ט טבת</t>
@@ -721,7 +721,7 @@
     <t>13/12</t>
   </si>
   <si>
-    <t>מלכ'א א מח</t>
+    <t>מלכ'א ב מה</t>
   </si>
   <si>
     <t>י טבת</t>
@@ -733,7 +733,7 @@
     <t>צום י טבת</t>
   </si>
   <si>
-    <t>מלכ'א ב מה</t>
+    <t>מלכ'א ד כ</t>
   </si>
   <si>
     <t>יא טבת</t>
@@ -742,7 +742,7 @@
     <t>15/12</t>
   </si>
   <si>
-    <t>מלכ'א ד כ</t>
+    <t>מלכ'א ו יג</t>
   </si>
   <si>
     <t>יב טבת</t>
@@ -751,7 +751,7 @@
     <t>16/12</t>
   </si>
   <si>
-    <t>מלכ'א ו יג</t>
+    <t>מלכ'א ז כא</t>
   </si>
   <si>
     <t>יג טבת</t>
@@ -760,7 +760,7 @@
     <t>17/12</t>
   </si>
   <si>
-    <t>מלכ'א ז כא</t>
+    <t>מלכ'א ח יא</t>
   </si>
   <si>
     <t>יד טבת</t>
@@ -778,7 +778,7 @@
     <t>19/12</t>
   </si>
   <si>
-    <t>מלכ'א ח יא</t>
+    <t>מלכ'א ח נח</t>
   </si>
   <si>
     <t>טז טבת</t>
@@ -787,7 +787,7 @@
     <t>20/12</t>
   </si>
   <si>
-    <t>מלכ'א ח נח</t>
+    <t>מלכ'א י ט</t>
   </si>
   <si>
     <t>יז טבת</t>
@@ -796,7 +796,7 @@
     <t>21/12</t>
   </si>
   <si>
-    <t>מלכ'א י ט</t>
+    <t>מלכ'א יא כח</t>
   </si>
   <si>
     <t>יח טבת</t>
@@ -805,7 +805,7 @@
     <t>22/12</t>
   </si>
   <si>
-    <t>מלכ'א יא כח</t>
+    <t>מלכ'א יב כד</t>
   </si>
   <si>
     <t>יט טבת</t>
@@ -814,7 +814,7 @@
     <t>23/12</t>
   </si>
   <si>
-    <t>מלכ'א יב כד</t>
+    <t>מלכ'א יג לא</t>
   </si>
   <si>
     <t>כ טבת</t>
@@ -823,7 +823,7 @@
     <t>24/12</t>
   </si>
   <si>
-    <t>מלכ'א יג לא</t>
+    <t>מלכ'א טו ח</t>
   </si>
   <si>
     <t>כא טבת</t>
@@ -841,7 +841,7 @@
     <t>26/12</t>
   </si>
   <si>
-    <t>מלכ'א טו ח</t>
+    <t>מלכ'א טז טו</t>
   </si>
   <si>
     <t>כג טבת</t>
@@ -850,7 +850,7 @@
     <t>27/12</t>
   </si>
   <si>
-    <t>מלכ'א טז טו</t>
+    <t>מלכ'א יז כד</t>
   </si>
   <si>
     <t>כד טבת</t>
@@ -859,7 +859,7 @@
     <t>28/12</t>
   </si>
   <si>
-    <t>מלכ'א יז כד</t>
+    <t>מלכ'א יח לט</t>
   </si>
   <si>
     <t>כה טבת</t>
@@ -868,7 +868,7 @@
     <t>29/12</t>
   </si>
   <si>
-    <t>מלכ'א יח לט</t>
+    <t>מלכ'א כ יג</t>
   </si>
   <si>
     <t>כו טבת</t>
@@ -877,7 +877,7 @@
     <t>30/12</t>
   </si>
   <si>
-    <t>מלכ'א כ יג</t>
+    <t>מלכ'א כא יח</t>
   </si>
   <si>
     <t>כז טבת</t>
@@ -886,7 +886,7 @@
     <t>31/12</t>
   </si>
   <si>
-    <t>מלכ'א כא יח</t>
+    <t>מלכ'א כב מג</t>
   </si>
   <si>
     <t>כח טבת</t>
@@ -904,7 +904,7 @@
     <t>2/1</t>
   </si>
   <si>
-    <t>מלכ'א כב מג</t>
+    <t>מלכ'ב ב טו</t>
   </si>
   <si>
     <t>א שבט</t>
@@ -913,7 +913,7 @@
     <t>3/1</t>
   </si>
   <si>
-    <t>מלכ'ב ב טו</t>
+    <t>מלכ'ב ד כו</t>
   </si>
   <si>
     <t>ב שבט</t>
@@ -922,7 +922,7 @@
     <t>4/1</t>
   </si>
   <si>
-    <t>מלכ'ב ד כו</t>
+    <t>מלכ'ב ו כג</t>
   </si>
   <si>
     <t>ג שבט</t>
@@ -931,7 +931,7 @@
     <t>5/1</t>
   </si>
   <si>
-    <t>מלכ'ב ו כג</t>
+    <t>מלכ'ב ז טז</t>
   </si>
   <si>
     <t>ד שבט</t>
@@ -940,7 +940,7 @@
     <t>6/1</t>
   </si>
   <si>
-    <t>מלכ'ב ז טז</t>
+    <t>מלכ'ב ט יג</t>
   </si>
   <si>
     <t>ה שבט</t>
@@ -949,7 +949,7 @@
     <t>7/1</t>
   </si>
   <si>
-    <t>מלכ'ב ט יג</t>
+    <t>מלכ'ב י טו</t>
   </si>
   <si>
     <t>ו שבט</t>
@@ -967,7 +967,7 @@
     <t>9/1</t>
   </si>
   <si>
-    <t>מלכ'ב י טו</t>
+    <t>מלכ'ב יב ג</t>
   </si>
   <si>
     <t>ח שבט</t>
@@ -976,7 +976,7 @@
     <t>10/1</t>
   </si>
   <si>
-    <t>מלכ'ב יב ג</t>
+    <t>מלכ'ב יג כג</t>
   </si>
   <si>
     <t>ט שבט</t>
@@ -985,7 +985,7 @@
     <t>11/1</t>
   </si>
   <si>
-    <t>מלכ'ב יג כג</t>
+    <t>מלכ'ב טו ז</t>
   </si>
   <si>
     <t>י שבט</t>
@@ -994,7 +994,7 @@
     <t>12/1</t>
   </si>
   <si>
-    <t>מלכ'ב טו ז</t>
+    <t>מלכ'ב טז כ</t>
   </si>
   <si>
     <t>יא שבט</t>
@@ -1003,7 +1003,7 @@
     <t>13/1</t>
   </si>
   <si>
-    <t>מלכ'ב טז כ</t>
+    <t>מלכ'ב יח ו</t>
   </si>
   <si>
     <t>יב שבט</t>
@@ -1012,7 +1012,7 @@
     <t>14/1</t>
   </si>
   <si>
-    <t>מלכ'ב יח ו</t>
+    <t>מלכ'ב יט יט</t>
   </si>
   <si>
     <t>יג שבט</t>
@@ -1030,7 +1030,7 @@
     <t>16/1</t>
   </si>
   <si>
-    <t>מלכ'ב יט יט</t>
+    <t>מלכ'ב כ ח</t>
   </si>
   <si>
     <t>טו שבט</t>
@@ -1042,7 +1042,7 @@
     <t>רה"ש לאילנות</t>
   </si>
   <si>
-    <t>מלכ'ב כ ח</t>
+    <t>מלכ'ב כב ב</t>
   </si>
   <si>
     <t>טז שבט</t>
@@ -1051,7 +1051,7 @@
     <t>18/1</t>
   </si>
   <si>
-    <t>מלכ'ב כב ב</t>
+    <t>מלכ'ב כג כה</t>
   </si>
   <si>
     <t>יז שבט</t>
@@ -1060,7 +1060,7 @@
     <t>19/1</t>
   </si>
   <si>
-    <t>מלכ'ב כג כה</t>
+    <t>מלכ'ב כד יח</t>
   </si>
   <si>
     <t>יח שבט</t>
@@ -1069,7 +1069,7 @@
     <t>20/1</t>
   </si>
   <si>
-    <t>מלכ'ב כד יח</t>
+    <t>ישעיהו א א</t>
   </si>
   <si>
     <t>יט שבט</t>
@@ -1078,7 +1078,7 @@
     <t>21/1</t>
   </si>
   <si>
-    <t>ישעיהו א א</t>
+    <t>ישעיהו ד ג</t>
   </si>
   <si>
     <t>כ שבט</t>
@@ -1096,7 +1096,7 @@
     <t>23/1</t>
   </si>
   <si>
-    <t>ישעיהו ד ג</t>
+    <t>ישעיהו ו ג</t>
   </si>
   <si>
     <t>כב שבט</t>
@@ -1105,7 +1105,7 @@
     <t>24/1</t>
   </si>
   <si>
-    <t>ישעיהו ו ג</t>
+    <t>ישעיהו ט ו</t>
   </si>
   <si>
     <t>כג שבט</t>
@@ -1114,7 +1114,7 @@
     <t>25/1</t>
   </si>
   <si>
-    <t>ישעיהו ט ו</t>
+    <t>ישעיהו יא ב</t>
   </si>
   <si>
     <t>כד שבט</t>
@@ -1123,7 +1123,7 @@
     <t>26/1</t>
   </si>
   <si>
-    <t>ישעיהו יא ב</t>
+    <t>ישעיהו יד ב</t>
   </si>
   <si>
     <t>כה שבט</t>
@@ -1132,7 +1132,7 @@
     <t>27/1</t>
   </si>
   <si>
-    <t>ישעיהו יד ב</t>
+    <t>ישעיהו טז ה</t>
   </si>
   <si>
     <t>כו שבט</t>
@@ -1141,7 +1141,7 @@
     <t>28/1</t>
   </si>
   <si>
-    <t>ישעיהו טז ה</t>
+    <t>ישעיהו יט כה</t>
   </si>
   <si>
     <t>כז שבט</t>
@@ -1159,7 +1159,7 @@
     <t>30/1</t>
   </si>
   <si>
-    <t>ישעיהו יט כה</t>
+    <t>ישעיהו כב כג</t>
   </si>
   <si>
     <t>כט שבט</t>
@@ -1168,7 +1168,7 @@
     <t>31/1</t>
   </si>
   <si>
-    <t>ישעיהו כב כג</t>
+    <t>ישעיהו כד כג</t>
   </si>
   <si>
     <t>ל שבט</t>
@@ -1177,7 +1177,7 @@
     <t>1/2</t>
   </si>
   <si>
-    <t>ישעיהו כד כג</t>
+    <t>ישעיהו כז יב</t>
   </si>
   <si>
     <t>א אדר א'</t>
@@ -1186,7 +1186,7 @@
     <t>2/2</t>
   </si>
   <si>
-    <t>ישעיהו כז יב</t>
+    <t>ישעיהו כט כג</t>
   </si>
   <si>
     <t>ב אדר א'</t>
@@ -1195,7 +1195,7 @@
     <t>3/2</t>
   </si>
   <si>
-    <t>ישעיהו כט כג</t>
+    <t>ישעיהו לב יח</t>
   </si>
   <si>
     <t>ג אדר א'</t>
@@ -1204,7 +1204,7 @@
     <t>4/2</t>
   </si>
   <si>
-    <t>ישעיהו לב יח</t>
+    <t>ישעיהו לה י</t>
   </si>
   <si>
     <t>ד אדר א'</t>
@@ -1222,7 +1222,7 @@
     <t>6/2</t>
   </si>
   <si>
-    <t>ישעיהו לה י</t>
+    <t>ישעיהו לז כ</t>
   </si>
   <si>
     <t>ו אדר א'</t>
@@ -1231,7 +1231,7 @@
     <t>7/2</t>
   </si>
   <si>
-    <t>ישעיהו לז כ</t>
+    <t>ישעיהו מ א</t>
   </si>
   <si>
     <t>ז אדר א'</t>
@@ -1240,7 +1240,7 @@
     <t>8/2</t>
   </si>
   <si>
-    <t>ישעיהו מ א</t>
+    <t>ישעיהו מא כז</t>
   </si>
   <si>
     <t>ח אדר א'</t>
@@ -1249,7 +1249,7 @@
     <t>9/2</t>
   </si>
   <si>
-    <t>ישעיהו מא כז</t>
+    <t>ישעיהו מד ו</t>
   </si>
   <si>
     <t>ט אדר א'</t>
@@ -1258,7 +1258,7 @@
     <t>10/2</t>
   </si>
   <si>
-    <t>ישעיהו מד ו</t>
+    <t>ישעיהו מה יז</t>
   </si>
   <si>
     <t>י אדר א'</t>
@@ -1267,7 +1267,7 @@
     <t>11/2</t>
   </si>
   <si>
-    <t>ישעיהו מה יז</t>
+    <t>ישעיהו מח ב</t>
   </si>
   <si>
     <t>יא אדר א'</t>
@@ -1285,7 +1285,7 @@
     <t>13/2</t>
   </si>
   <si>
-    <t>ישעיהו מח ב</t>
+    <t>ישעיהו מט כו</t>
   </si>
   <si>
     <t>יג אדר א'</t>
@@ -1294,7 +1294,7 @@
     <t>14/2</t>
   </si>
   <si>
-    <t>ישעיהו מט כו</t>
+    <t>ישעיהו נב ז</t>
   </si>
   <si>
     <t>יד אדר א'</t>
@@ -1306,7 +1306,7 @@
     <t>פורים קטן</t>
   </si>
   <si>
-    <t>ישעיהו נב ז</t>
+    <t>ישעיהו נה יג</t>
   </si>
   <si>
     <t>טו אדר א'</t>
@@ -1318,7 +1318,7 @@
     <t>שושן פורים קטן</t>
   </si>
   <si>
-    <t>ישעיהו נה יג</t>
+    <t>ישעיהו נח יד</t>
   </si>
   <si>
     <t>טז אדר א'</t>
@@ -1327,7 +1327,7 @@
     <t>17/2</t>
   </si>
   <si>
-    <t>ישעיהו נח יד</t>
+    <t>ישעיהו סא ט</t>
   </si>
   <si>
     <t>יז אדר א'</t>
@@ -1336,7 +1336,7 @@
     <t>18/2</t>
   </si>
   <si>
-    <t>ישעיהו סא ט</t>
+    <t>ישעיהו סה ט</t>
   </si>
   <si>
     <t>יח אדר א'</t>
@@ -1354,7 +1354,7 @@
     <t>20/2</t>
   </si>
   <si>
-    <t>ישעיהו סה ט</t>
+    <t>ירמיהו א א</t>
   </si>
   <si>
     <t>כ אדר א'</t>
@@ -1363,7 +1363,7 @@
     <t>21/2</t>
   </si>
   <si>
-    <t>ירמיהו א א</t>
+    <t>ירמיהו ג ד</t>
   </si>
   <si>
     <t>כא אדר א'</t>
@@ -1372,7 +1372,7 @@
     <t>22/2</t>
   </si>
   <si>
-    <t>ירמיהו ג ד</t>
+    <t>ירמיהו ה א</t>
   </si>
   <si>
     <t>כב אדר א'</t>
@@ -1381,7 +1381,7 @@
     <t>23/2</t>
   </si>
   <si>
-    <t>ירמיהו ה א</t>
+    <t>ירמיהו ו ג</t>
   </si>
   <si>
     <t>כג אדר א'</t>
@@ -1390,7 +1390,7 @@
     <t>24/2</t>
   </si>
   <si>
-    <t>ירמיהו ו ג</t>
+    <t>ירמיהו ז כג</t>
   </si>
   <si>
     <t>כד אדר א'</t>
@@ -1399,7 +1399,7 @@
     <t>25/2</t>
   </si>
   <si>
-    <t>ירמיהו ז כג</t>
+    <t>ירמיהו ט כג</t>
   </si>
   <si>
     <t>כה אדר א'</t>
@@ -1417,7 +1417,7 @@
     <t>27/2</t>
   </si>
   <si>
-    <t>ירמיהו ט כג</t>
+    <t>ירמיהו יב טו</t>
   </si>
   <si>
     <t>כז אדר א'</t>
@@ -1426,7 +1426,7 @@
     <t>28/2</t>
   </si>
   <si>
-    <t>ירמיהו יב טו</t>
+    <t>ירמיהו יד כב</t>
   </si>
   <si>
     <t>כח אדר א'</t>
@@ -1435,7 +1435,7 @@
     <t>1/3</t>
   </si>
   <si>
-    <t>ירמיהו יד כב</t>
+    <t>ירמיהו יז ז</t>
   </si>
   <si>
     <t>כט אדר א'</t>
@@ -1444,7 +1444,7 @@
     <t>2/3</t>
   </si>
   <si>
-    <t>ירמיהו יז ז</t>
+    <t>ירמיהו יח יט</t>
   </si>
   <si>
     <t>ל אדר א'</t>
@@ -1453,7 +1453,7 @@
     <t>3/3</t>
   </si>
   <si>
-    <t>ירמיהו יח יט</t>
+    <t>ירמיהו כ יג</t>
   </si>
   <si>
     <t>א אדר ב'</t>
@@ -1462,7 +1462,7 @@
     <t>4/3</t>
   </si>
   <si>
-    <t>ירמיהו כ יג</t>
+    <t>ירמיהו כג ו</t>
   </si>
   <si>
     <t>ב אדר ב'</t>
@@ -1480,7 +1480,7 @@
     <t>6/3</t>
   </si>
   <si>
-    <t>ירמיהו כג ו</t>
+    <t>ירמיהו כד ז</t>
   </si>
   <si>
     <t>ד אדר ב'</t>
@@ -1489,7 +1489,7 @@
     <t>7/3</t>
   </si>
   <si>
-    <t>ירמיהו כד ז</t>
+    <t>ירמיהו כו א</t>
   </si>
   <si>
     <t>ה אדר ב'</t>
@@ -1498,7 +1498,7 @@
     <t>8/3</t>
   </si>
   <si>
-    <t>ירמיהו כו א</t>
+    <t>ירמיהו כז ה</t>
   </si>
   <si>
     <t>ו אדר ב'</t>
@@ -1507,7 +1507,7 @@
     <t>9/3</t>
   </si>
   <si>
-    <t>ירמיהו כז ה</t>
+    <t>ירמיהו כט ז</t>
   </si>
   <si>
     <t>ז אדר ב'</t>
@@ -1516,7 +1516,7 @@
     <t>10/3</t>
   </si>
   <si>
-    <t>ירמיהו כט ז</t>
+    <t>ירמיהו ל ט</t>
   </si>
   <si>
     <t>ח אדר ב'</t>
@@ -1525,7 +1525,7 @@
     <t>11/3</t>
   </si>
   <si>
-    <t>ירמיהו ל ט</t>
+    <t>ירמיהו לא לב</t>
   </si>
   <si>
     <t>ט אדר ב'</t>
@@ -1543,7 +1543,7 @@
     <t>13/3</t>
   </si>
   <si>
-    <t>ירמיהו לא לב</t>
+    <t>ירמיהו לב כב</t>
   </si>
   <si>
     <t>יא אדר ב'</t>
@@ -1552,7 +1552,7 @@
     <t>14/3</t>
   </si>
   <si>
-    <t>ירמיהו לב כב</t>
+    <t>ירמיהו לג טז</t>
   </si>
   <si>
     <t>יב אדר ב'</t>
@@ -1561,7 +1561,7 @@
     <t>15/3</t>
   </si>
   <si>
-    <t>ירמיהו לג טז</t>
+    <t>ירמיהו לה י</t>
   </si>
   <si>
     <t>יג אדר ב'</t>
@@ -1573,7 +1573,7 @@
     <t>תענית אסתר</t>
   </si>
   <si>
-    <t>ירמיהו לה י</t>
+    <t>ירמיהו לו כו</t>
   </si>
   <si>
     <t>יד אדר ב'</t>
@@ -1594,7 +1594,7 @@
     <t>שושן פורים</t>
   </si>
   <si>
-    <t>ירמיהו לו כו</t>
+    <t>ירמיהו לח ח</t>
   </si>
   <si>
     <t>טז אדר ב'</t>
@@ -1612,7 +1612,7 @@
     <t>20/3</t>
   </si>
   <si>
-    <t>ירמיהו לח ח</t>
+    <t>ירמיהו לט יח</t>
   </si>
   <si>
     <t>יח אדר ב'</t>
@@ -1621,7 +1621,7 @@
     <t>21/3</t>
   </si>
   <si>
-    <t>ירמיהו לט יח</t>
+    <t>ירמיהו מב יב</t>
   </si>
   <si>
     <t>יט אדר ב'</t>
@@ -1630,7 +1630,7 @@
     <t>22/3</t>
   </si>
   <si>
-    <t>ירמיהו מב יב</t>
+    <t>ירמיהו מד כ</t>
   </si>
   <si>
     <t>כ אדר ב'</t>
@@ -1639,7 +1639,7 @@
     <t>23/3</t>
   </si>
   <si>
-    <t>ירמיהו מד כ</t>
+    <t>ירמיהו מו כז</t>
   </si>
   <si>
     <t>כא אדר ב'</t>
@@ -1648,7 +1648,7 @@
     <t>24/3</t>
   </si>
   <si>
-    <t>ירמיהו מו כז</t>
+    <t>ירמיהו מט ב</t>
   </si>
   <si>
     <t>כב אדר ב'</t>
@@ -1657,7 +1657,7 @@
     <t>25/3</t>
   </si>
   <si>
-    <t>ירמיהו מט ב</t>
+    <t>ירמיהו נ ה</t>
   </si>
   <si>
     <t>כג אדר ב'</t>
@@ -1675,7 +1675,7 @@
     <t>27/3</t>
   </si>
   <si>
-    <t>ירמיהו נ ה</t>
+    <t>ירמיהו נא י</t>
   </si>
   <si>
     <t>כה אדר ב'</t>
@@ -1684,7 +1684,7 @@
     <t>28/3</t>
   </si>
   <si>
-    <t>ירמיהו נא י</t>
+    <t>ירמיהו נא נט</t>
   </si>
   <si>
     <t>כו אדר ב'</t>
@@ -1693,7 +1693,7 @@
     <t>29/3</t>
   </si>
   <si>
-    <t>ירמיהו נא נט</t>
+    <t>יחזקאל א א</t>
   </si>
   <si>
     <t>כז אדר ב'</t>
@@ -1702,7 +1702,7 @@
     <t>30/3</t>
   </si>
   <si>
-    <t>יחזקאל א א</t>
+    <t>יחזקאל ג יב</t>
   </si>
   <si>
     <t>כח אדר ב'</t>
@@ -1711,7 +1711,7 @@
     <t>31/3</t>
   </si>
   <si>
-    <t>יחזקאל ג יב</t>
+    <t>יחזקאל ו א</t>
   </si>
   <si>
     <t>כט אדר ב'</t>
@@ -1720,7 +1720,7 @@
     <t>1/4</t>
   </si>
   <si>
-    <t>יחזקאל ו א</t>
+    <t>יחזקאל ח א</t>
   </si>
   <si>
     <t>א ניסן</t>
@@ -1738,7 +1738,7 @@
     <t>3/4</t>
   </si>
   <si>
-    <t>יחזקאל ח א</t>
+    <t>יחזקאל י א</t>
   </si>
   <si>
     <t>ג ניסן</t>
@@ -1747,7 +1747,7 @@
     <t>4/4</t>
   </si>
   <si>
-    <t>יחזקאל י א</t>
+    <t>יחזקאל יא כ</t>
   </si>
   <si>
     <t>ד ניסן</t>
@@ -1756,7 +1756,7 @@
     <t>5/4</t>
   </si>
   <si>
-    <t>יחזקאל יא כ</t>
+    <t>יחזקאל יד א</t>
   </si>
   <si>
     <t>ה ניסן</t>
@@ -1765,7 +1765,7 @@
     <t>6/4</t>
   </si>
   <si>
-    <t>יחזקאל יד א</t>
+    <t>יחזקאל טז יד</t>
   </si>
   <si>
     <t>ו ניסן</t>
@@ -1774,7 +1774,7 @@
     <t>7/4</t>
   </si>
   <si>
-    <t>יחזקאל טז יד</t>
+    <t>יחזקאל טז ס</t>
   </si>
   <si>
     <t>ז ניסן</t>
@@ -1783,7 +1783,7 @@
     <t>8/4</t>
   </si>
   <si>
-    <t>יחזקאל טז ס</t>
+    <t>יחזקאל יח ט</t>
   </si>
   <si>
     <t>ח ניסן</t>
@@ -1801,7 +1801,7 @@
     <t>10/4</t>
   </si>
   <si>
-    <t>יחזקאל יח ט</t>
+    <t>יחזקאל כ א</t>
   </si>
   <si>
     <t>י ניסן</t>
@@ -1810,7 +1810,7 @@
     <t>11/4</t>
   </si>
   <si>
-    <t>יחזקאל כ א</t>
+    <t>יחזקאל כ מא</t>
   </si>
   <si>
     <t>יא ניסן</t>
@@ -1819,7 +1819,7 @@
     <t>12/4</t>
   </si>
   <si>
-    <t>יחזקאל כ מא</t>
+    <t>יחזקאל כב טז</t>
   </si>
   <si>
     <t>יב ניסן</t>
@@ -1828,7 +1828,7 @@
     <t>13/4</t>
   </si>
   <si>
-    <t>יחזקאל כב טז</t>
+    <t>יחזקאל כג כז</t>
   </si>
   <si>
     <t>יג ניסן</t>
@@ -1837,7 +1837,7 @@
     <t>14/4</t>
   </si>
   <si>
-    <t>יחזקאל כג כז</t>
+    <t>יחזקאל כד כד</t>
   </si>
   <si>
     <t>יד ניסן</t>
@@ -1846,7 +1846,7 @@
     <t>15/4</t>
   </si>
   <si>
-    <t>יחזקאל כד כד</t>
+    <t>יחזקאל כו כ</t>
   </si>
   <si>
     <t>טו ניסן</t>
@@ -1867,7 +1867,7 @@
     <t>חוה"מ</t>
   </si>
   <si>
-    <t>יחזקאל כו כ</t>
+    <t>יחזקאל כח יג</t>
   </si>
   <si>
     <t>יז ניסן</t>
@@ -1876,7 +1876,7 @@
     <t>18/4</t>
   </si>
   <si>
-    <t>יחזקאל כח יג</t>
+    <t>יחזקאל כט כא</t>
   </si>
   <si>
     <t>יח ניסן</t>
@@ -1885,7 +1885,7 @@
     <t>19/4</t>
   </si>
   <si>
-    <t>יחזקאל כט כא</t>
+    <t>יחזקאל לב א</t>
   </si>
   <si>
     <t>יט ניסן</t>
@@ -1894,7 +1894,7 @@
     <t>20/4</t>
   </si>
   <si>
-    <t>יחזקאל לב א</t>
+    <t>יחזקאל לג טז</t>
   </si>
   <si>
     <t>כ ניסן</t>
@@ -1903,7 +1903,7 @@
     <t>21/4</t>
   </si>
   <si>
-    <t>יחזקאל לג טז</t>
+    <t>יחזקאל לד כו</t>
   </si>
   <si>
     <t>כא ניסן</t>
@@ -1930,7 +1930,7 @@
     <t>24/4</t>
   </si>
   <si>
-    <t>יחזקאל לד כו</t>
+    <t>יחזקאל לו כה</t>
   </si>
   <si>
     <t>כד ניסן</t>
@@ -1939,7 +1939,7 @@
     <t>25/4</t>
   </si>
   <si>
-    <t>יחזקאל לו כה</t>
+    <t>יחזקאל לז כח</t>
   </si>
   <si>
     <t>כה ניסן</t>
@@ -1948,7 +1948,7 @@
     <t>26/4</t>
   </si>
   <si>
-    <t>יחזקאל לז כח</t>
+    <t>יחזקאל לט כב</t>
   </si>
   <si>
     <t>כו ניסן</t>
@@ -1957,7 +1957,7 @@
     <t>27/4</t>
   </si>
   <si>
-    <t>יחזקאל לט כב</t>
+    <t>יחזקאל מ מה</t>
   </si>
   <si>
     <t>כז ניסן</t>
@@ -1966,7 +1966,7 @@
     <t>28/4</t>
   </si>
   <si>
-    <t>יחזקאל מ מה</t>
+    <t>יחזקאל מב יג</t>
   </si>
   <si>
     <t>כח ניסן</t>
@@ -1975,7 +1975,7 @@
     <t>29/4</t>
   </si>
   <si>
-    <t>יחזקאל מב יג</t>
+    <t>יחזקאל מג כז</t>
   </si>
   <si>
     <t>כט ניסן</t>
@@ -1993,7 +1993,7 @@
     <t>1/5</t>
   </si>
   <si>
-    <t>יחזקאל מג כז</t>
+    <t>יחזקאל מה טו</t>
   </si>
   <si>
     <t>א אייר</t>
@@ -2002,7 +2002,7 @@
     <t>2/5</t>
   </si>
   <si>
-    <t>יחזקאל מה טו</t>
+    <t>יחזקאל מז יב</t>
   </si>
   <si>
     <t>ב אייר</t>
@@ -2011,7 +2011,7 @@
     <t>3/5</t>
   </si>
   <si>
-    <t>יחזקאל מז יב</t>
+    <t>הושע א א</t>
   </si>
   <si>
     <t>ג אייר</t>
@@ -2023,7 +2023,7 @@
     <t>יום הזיכרון</t>
   </si>
   <si>
-    <t>הושע א א</t>
+    <t>הושע ו ב</t>
   </si>
   <si>
     <t>ד אייר</t>
@@ -2041,7 +2041,7 @@
     <t>6/5</t>
   </si>
   <si>
-    <t>הושע ו ב</t>
+    <t>הושע י יב</t>
   </si>
   <si>
     <t>ו אייר</t>
@@ -2059,7 +2059,7 @@
     <t>8/5</t>
   </si>
   <si>
-    <t>הושע י יב</t>
+    <t>הושע יד ו</t>
   </si>
   <si>
     <t>ח אייר</t>
@@ -2068,7 +2068,7 @@
     <t>9/5</t>
   </si>
   <si>
-    <t>הושע יד ו</t>
+    <t>יואל ב כז</t>
   </si>
   <si>
     <t>ט אייר</t>
@@ -2077,7 +2077,7 @@
     <t>10/5</t>
   </si>
   <si>
-    <t>יואל ב כז</t>
+    <t>עמוס ב י</t>
   </si>
   <si>
     <t>י אייר</t>
@@ -2086,7 +2086,7 @@
     <t>11/5</t>
   </si>
   <si>
-    <t>עמוס ב י</t>
+    <t>עמוס ה יד</t>
   </si>
   <si>
     <t>יא אייר</t>
@@ -2095,7 +2095,7 @@
     <t>12/5</t>
   </si>
   <si>
-    <t>עמוס ה יד</t>
+    <t>עמוס ז טו</t>
   </si>
   <si>
     <t>יב אייר</t>
@@ -2104,7 +2104,7 @@
     <t>13/5</t>
   </si>
   <si>
-    <t>עמוס ז טו</t>
+    <t>עובדיה א כא</t>
   </si>
   <si>
     <t>יג אייר</t>
@@ -2122,7 +2122,7 @@
     <t>15/5</t>
   </si>
   <si>
-    <t>עובדיה א כא</t>
+    <t>מיכה א א</t>
   </si>
   <si>
     <t>טו אייר</t>
@@ -2131,7 +2131,7 @@
     <t>16/5</t>
   </si>
   <si>
-    <t>מיכה א א</t>
+    <t>מיכה ד ה</t>
   </si>
   <si>
     <t>טז אייר</t>
@@ -2140,7 +2140,7 @@
     <t>17/5</t>
   </si>
   <si>
-    <t>מיכה ד ה</t>
+    <t>מיכה ז כ</t>
   </si>
   <si>
     <t>יז אייר</t>
@@ -2149,7 +2149,7 @@
     <t>18/5</t>
   </si>
   <si>
-    <t>מיכה ז כ</t>
+    <t>חבקוק א א</t>
   </si>
   <si>
     <t>יח אייר</t>
@@ -2158,7 +2158,7 @@
     <t>19/5</t>
   </si>
   <si>
-    <t>חבקוק א א</t>
+    <t>צפניה א א</t>
   </si>
   <si>
     <t>יט אייר</t>
@@ -2167,7 +2167,7 @@
     <t>20/5</t>
   </si>
   <si>
-    <t>צפניה א א</t>
+    <t>צפניה ג כ</t>
   </si>
   <si>
     <t>כ אייר</t>
@@ -2185,7 +2185,7 @@
     <t>22/5</t>
   </si>
   <si>
-    <t>צפניה ג כ</t>
+    <t>חגי ב כג</t>
   </si>
   <si>
     <t>כב אייר</t>
@@ -2194,7 +2194,7 @@
     <t>23/5</t>
   </si>
   <si>
-    <t>חגי ב כג</t>
+    <t>זכריה ד ב</t>
   </si>
   <si>
     <t>כג אייר</t>
@@ -2203,7 +2203,7 @@
     <t>24/5</t>
   </si>
   <si>
-    <t>זכריה ד ב</t>
+    <t>זכריה ו יד</t>
   </si>
   <si>
     <t>כד אייר</t>
@@ -2212,7 +2212,7 @@
     <t>25/5</t>
   </si>
   <si>
-    <t>זכריה ו יד</t>
+    <t>זכריה ח כג</t>
   </si>
   <si>
     <t>כה אייר</t>
@@ -2221,7 +2221,7 @@
     <t>26/5</t>
   </si>
   <si>
-    <t>זכריה ח כג</t>
+    <t>זכריה יב א</t>
   </si>
   <si>
     <t>כו אייר</t>
@@ -2230,7 +2230,7 @@
     <t>27/5</t>
   </si>
   <si>
-    <t>זכריה יב א</t>
+    <t>זכריה יד כא</t>
   </si>
   <si>
     <t>כז אייר</t>
@@ -2248,7 +2248,7 @@
     <t>29/5</t>
   </si>
   <si>
-    <t>זכריה יד כא</t>
+    <t>תהלים א א</t>
   </si>
   <si>
     <t>כט אייר</t>
@@ -2257,7 +2257,7 @@
     <t>30/5</t>
   </si>
   <si>
-    <t>תהלים א א</t>
+    <t>תהלים יא ז</t>
   </si>
   <si>
     <t>א סיון</t>
@@ -2266,7 +2266,7 @@
     <t>31/5</t>
   </si>
   <si>
-    <t>תהלים יא ז</t>
+    <t>תהלים כ י</t>
   </si>
   <si>
     <t>ב סיון</t>
@@ -2275,7 +2275,7 @@
     <t>1/6</t>
   </si>
   <si>
-    <t>תהלים כ י</t>
+    <t>תהלים כט יא</t>
   </si>
   <si>
     <t>ג סיון</t>
@@ -2284,7 +2284,7 @@
     <t>2/6</t>
   </si>
   <si>
-    <t>תהלים כט יא</t>
+    <t>תהלים לה כח</t>
   </si>
   <si>
     <t>ד סיון</t>
@@ -2293,7 +2293,7 @@
     <t>3/6</t>
   </si>
   <si>
-    <t>תהלים לה כח</t>
+    <t>תהלים מא יד</t>
   </si>
   <si>
     <t>ה סיון</t>
@@ -2320,7 +2320,7 @@
     <t>6/6</t>
   </si>
   <si>
-    <t>תהלים מא יד</t>
+    <t>תהלים מט יט</t>
   </si>
   <si>
     <t>ח סיון</t>
@@ -2329,7 +2329,7 @@
     <t>7/6</t>
   </si>
   <si>
-    <t>תהלים מט יט</t>
+    <t>תהלים נז יב</t>
   </si>
   <si>
     <t>ט סיון</t>
@@ -2338,7 +2338,7 @@
     <t>8/6</t>
   </si>
   <si>
-    <t>תהלים נז יב</t>
+    <t>תהלים סז ח</t>
   </si>
   <si>
     <t>י סיון</t>
@@ -2347,7 +2347,7 @@
     <t>9/6</t>
   </si>
   <si>
-    <t>תהלים סז ח</t>
+    <t>תהלים עב כ</t>
   </si>
   <si>
     <t>יא סיון</t>
@@ -2356,7 +2356,7 @@
     <t>10/6</t>
   </si>
   <si>
-    <t>תהלים עב כ</t>
+    <t>תהלים עח לח</t>
   </si>
   <si>
     <t>יב סיון</t>
@@ -2374,7 +2374,7 @@
     <t>12/6</t>
   </si>
   <si>
-    <t>תהלים עח לח</t>
+    <t>תהלים פד יג</t>
   </si>
   <si>
     <t>יד סיון</t>
@@ -2383,7 +2383,7 @@
     <t>13/6</t>
   </si>
   <si>
-    <t>תהלים פד יג</t>
+    <t>תהלים צ יז</t>
   </si>
   <si>
     <t>טו סיון</t>
@@ -2392,7 +2392,7 @@
     <t>14/6</t>
   </si>
   <si>
-    <t>תהלים צ יז</t>
+    <t>תהלים קא א</t>
   </si>
   <si>
     <t>טז סיון</t>
@@ -2401,7 +2401,7 @@
     <t>15/6</t>
   </si>
   <si>
-    <t>תהלים קא א</t>
+    <t>תהלים קה מה</t>
   </si>
   <si>
     <t>יז סיון</t>
@@ -2410,7 +2410,7 @@
     <t>16/6</t>
   </si>
   <si>
-    <t>תהלים קה מה</t>
+    <t>תהלים קיא י</t>
   </si>
   <si>
     <t>יח סיון</t>
@@ -2419,7 +2419,7 @@
     <t>17/6</t>
   </si>
   <si>
-    <t>תהלים קיא י</t>
+    <t>תהלים קיט עב</t>
   </si>
   <si>
     <t>יט סיון</t>
@@ -2437,7 +2437,7 @@
     <t>19/6</t>
   </si>
   <si>
-    <t>תהלים קיט עב</t>
+    <t>תהלים קכח ו</t>
   </si>
   <si>
     <t>כא סיון</t>
@@ -2446,7 +2446,7 @@
     <t>20/6</t>
   </si>
   <si>
-    <t>תהלים קכח ו</t>
+    <t>תהלים קמ יד</t>
   </si>
   <si>
     <t>כב סיון</t>
@@ -2455,7 +2455,7 @@
     <t>21/6</t>
   </si>
   <si>
-    <t>תהלים קמ יד</t>
+    <t>משלי א א</t>
   </si>
   <si>
     <t>כג סיון</t>
@@ -2464,7 +2464,7 @@
     <t>22/6</t>
   </si>
   <si>
-    <t>משלי א א</t>
+    <t>משלי ה יח</t>
   </si>
   <si>
     <t>כד סיון</t>
@@ -2473,7 +2473,7 @@
     <t>23/6</t>
   </si>
   <si>
-    <t>משלי ה יח</t>
+    <t>משלי ט יא</t>
   </si>
   <si>
     <t>כה סיון</t>
@@ -2482,7 +2482,7 @@
     <t>24/6</t>
   </si>
   <si>
-    <t>משלי ט יא</t>
+    <t>משלי יד ד</t>
   </si>
   <si>
     <t>כו סיון</t>
@@ -2500,7 +2500,7 @@
     <t>26/6</t>
   </si>
   <si>
-    <t>משלי יד ד</t>
+    <t>משלי יח י</t>
   </si>
   <si>
     <t>כח סיון</t>
@@ -2509,7 +2509,7 @@
     <t>27/6</t>
   </si>
   <si>
-    <t>משלי יח י</t>
+    <t>משלי כב כא</t>
   </si>
   <si>
     <t>כט סיון</t>
@@ -2518,7 +2518,7 @@
     <t>28/6</t>
   </si>
   <si>
-    <t>משלי כב כא</t>
+    <t>משלי כה יג</t>
   </si>
   <si>
     <t>ל סיון</t>
@@ -2527,7 +2527,7 @@
     <t>29/6</t>
   </si>
   <si>
-    <t>משלי כה יג</t>
+    <t>משלי כח טז</t>
   </si>
   <si>
     <t>א תמוז</t>
@@ -2536,7 +2536,7 @@
     <t>30/6</t>
   </si>
   <si>
-    <t>משלי כח טז</t>
+    <t>איוב א א</t>
   </si>
   <si>
     <t>ב תמוז</t>
@@ -2545,7 +2545,7 @@
     <t>1/7</t>
   </si>
   <si>
-    <t>איוב א א</t>
+    <t>איוב ה כז</t>
   </si>
   <si>
     <t>ג תמוז</t>
@@ -2563,7 +2563,7 @@
     <t>3/7</t>
   </si>
   <si>
-    <t>איוב ה כז</t>
+    <t>איוב יא יט</t>
   </si>
   <si>
     <t>ה תמוז</t>
@@ -2572,7 +2572,7 @@
     <t>4/7</t>
   </si>
   <si>
-    <t>איוב יא יט</t>
+    <t>איוב יז ט</t>
   </si>
   <si>
     <t>ו תמוז</t>
@@ -2581,7 +2581,7 @@
     <t>5/7</t>
   </si>
   <si>
-    <t>איוב יז ט</t>
+    <t>איוב כב ל</t>
   </si>
   <si>
     <t>ז תמוז</t>
@@ -2590,7 +2590,7 @@
     <t>6/7</t>
   </si>
   <si>
-    <t>איוב כב ל</t>
+    <t>איוב כט יד</t>
   </si>
   <si>
     <t>ח תמוז</t>
@@ -2599,7 +2599,7 @@
     <t>7/7</t>
   </si>
   <si>
-    <t>איוב כט יד</t>
+    <t>איוב לג לג</t>
   </si>
   <si>
     <t>ט תמוז</t>
@@ -2608,7 +2608,7 @@
     <t>8/7</t>
   </si>
   <si>
-    <t>איוב לג לג</t>
+    <t>איוב לח לה</t>
   </si>
   <si>
     <t>י תמוז</t>
@@ -2626,7 +2626,7 @@
     <t>10/7</t>
   </si>
   <si>
-    <t>איוב לח לה</t>
+    <t>שיר השירים א א</t>
   </si>
   <si>
     <t>יב תמוז</t>
@@ -2635,7 +2635,7 @@
     <t>11/7</t>
   </si>
   <si>
-    <t>שיר השירים א א</t>
+    <t>רות א א</t>
   </si>
   <si>
     <t>יג תמוז</t>
@@ -2644,7 +2644,7 @@
     <t>12/7</t>
   </si>
   <si>
-    <t>רות א א</t>
+    <t>רות ב יב</t>
   </si>
   <si>
     <t>יד תמוז</t>
@@ -3403,6 +3403,12 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="David"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -3411,12 +3417,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="David"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="David"/>
       <family val="1"/>
@@ -3499,6 +3499,8 @@
   <cellXfs count="17">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="1"/>
+    <xf applyFont="1" fontId="0" applyBorder="1" borderId="1"/>
+    <xf applyFont="1" fontId="1" applyBorder="1" borderId="1"/>
     <xf applyFont="1" fontId="2"/>
     <xf applyFont="1" fontId="3"/>
     <xf applyFont="1" fontId="0" applyAlignment="1">
@@ -3507,8 +3509,6 @@
     <xf applyFont="1" fontId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyFont="1" fontId="0" applyBorder="1" borderId="1"/>
-    <xf applyFont="1" fontId="3" applyBorder="1" borderId="1"/>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="2"/>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="3"/>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="4"/>
@@ -3516,10 +3516,10 @@
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="3" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf applyFont="1" fontId="3" applyBorder="1" borderId="4"/>
     <xf applyFont="1" fontId="2" applyBorder="1" borderId="4"/>
-    <xf applyFont="1" fontId="1" applyBorder="1" borderId="4"/>
-    <xf applyFont="1" fontId="1" applyBorder="1" borderId="5"/>
-    <xf applyFont="1" fontId="1" applyBorder="1" borderId="5" applyAlignment="1">
+    <xf applyFont="1" fontId="2" applyBorder="1" borderId="5"/>
+    <xf applyFont="1" fontId="2" applyBorder="1" borderId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3535,34 +3535,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="7"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="8" t="s">

</xml_diff>